<commit_message>
updated artefacts and requirements
</commit_message>
<xml_diff>
--- a/Project 3 Requirments.xlsx
+++ b/Project 3 Requirments.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="121">
   <si>
     <t>Reference Story No.</t>
   </si>
@@ -215,7 +215,7 @@
     <t>Create visuals for spaceship</t>
   </si>
   <si>
-    <t>Create the initial architecture document based off of Sprint 1</t>
+    <t>Create the visuals for the player</t>
   </si>
   <si>
     <t>Create visuals for asteroids</t>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>Create the Architecture Document</t>
+  </si>
+  <si>
+    <t>Create the initial architecture document based off of Sprint 1</t>
   </si>
   <si>
     <t>Deliver Packages between 2 points</t>
@@ -243,6 +246,12 @@
   </si>
   <si>
     <t>Create asteriods with resources the player can collect for resources</t>
+  </si>
+  <si>
+    <t>Camera Movement</t>
+  </si>
+  <si>
+    <t>Have the camera follow the player around and keep them on screen</t>
   </si>
   <si>
     <t>Create resource asteroid, package, and base visuals</t>
@@ -29318,7 +29327,7 @@
         <v>1.0</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -29346,7 +29355,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C11" s="15">
         <v>3.0</v>
@@ -29358,7 +29367,7 @@
         <v>2.0</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -29386,7 +29395,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C12" s="15">
         <v>2.0</v>
@@ -29398,7 +29407,7 @@
         <v>2.0</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -29426,7 +29435,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C13" s="15">
         <v>2.0</v>
@@ -29438,7 +29447,7 @@
         <v>2.0</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -29466,7 +29475,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="15">
         <v>3.0</v>
@@ -29478,7 +29487,7 @@
         <v>2.0</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -29506,19 +29515,19 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C15" s="15">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="D15" s="15">
         <v>2.0</v>
       </c>
       <c r="E15" s="15">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -29546,10 +29555,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C16" s="15">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D16" s="15">
         <v>2.0</v>
@@ -29558,7 +29567,7 @@
         <v>3.0</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -29586,10 +29595,10 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C17" s="15">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D17" s="15">
         <v>2.0</v>
@@ -29598,7 +29607,7 @@
         <v>3.0</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -29626,7 +29635,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" s="15">
         <v>1.0</v>
@@ -29638,7 +29647,7 @@
         <v>3.0</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -29666,7 +29675,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C19" s="15">
         <v>1.0</v>
@@ -29678,7 +29687,7 @@
         <v>3.0</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -29706,10 +29715,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C20" s="15">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D20" s="15">
         <v>2.0</v>
@@ -29718,7 +29727,7 @@
         <v>3.0</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
@@ -29746,10 +29755,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C21" s="15">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D21" s="15">
         <v>2.0</v>
@@ -29758,7 +29767,7 @@
         <v>3.0</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -29786,10 +29795,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C22" s="15">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="D22" s="15">
         <v>2.0</v>
@@ -29798,7 +29807,7 @@
         <v>3.0</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -29826,7 +29835,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C23" s="15">
         <v>5.0</v>
@@ -29834,8 +29843,8 @@
       <c r="D23" s="15">
         <v>2.0</v>
       </c>
-      <c r="E23" s="15" t="s">
-        <v>96</v>
+      <c r="E23" s="15">
+        <v>3.0</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>97</v>
@@ -29869,16 +29878,16 @@
         <v>98</v>
       </c>
       <c r="C24" s="15">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="D24" s="15">
         <v>2.0</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -29906,19 +29915,19 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C25" s="15">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="D25" s="15">
         <v>2.0</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -29946,19 +29955,19 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C26" s="15">
+        <v>5.0</v>
+      </c>
+      <c r="D26" s="15">
         <v>2.0</v>
       </c>
-      <c r="D26" s="15">
-        <v>1.0</v>
-      </c>
       <c r="E26" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -29986,19 +29995,19 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C27" s="15">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="D27" s="15">
         <v>1.0</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -30026,19 +30035,19 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C28" s="15">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="D28" s="15">
         <v>1.0</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
@@ -30066,19 +30075,19 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C29" s="15">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D29" s="15">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -30106,19 +30115,19 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C30" s="15">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="D30" s="15">
         <v>2.0</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -30146,19 +30155,19 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C31" s="15">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="D31" s="15">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -30186,19 +30195,19 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C32" s="15">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D32" s="15">
         <v>1.0</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
@@ -30226,19 +30235,19 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C33" s="15">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D33" s="15">
         <v>1.0</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -30262,12 +30271,24 @@
       <c r="Z33" s="9"/>
     </row>
     <row r="34">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
+      <c r="A34" s="10">
+        <v>33.0</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="D34" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>120</v>
+      </c>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -57449,6 +57470,34 @@
       <c r="Y1004" s="9"/>
       <c r="Z1004" s="9"/>
     </row>
+    <row r="1005">
+      <c r="A1005" s="9"/>
+      <c r="B1005" s="9"/>
+      <c r="C1005" s="9"/>
+      <c r="D1005" s="9"/>
+      <c r="E1005" s="9"/>
+      <c r="F1005" s="9"/>
+      <c r="G1005" s="9"/>
+      <c r="H1005" s="9"/>
+      <c r="I1005" s="9"/>
+      <c r="J1005" s="9"/>
+      <c r="K1005" s="9"/>
+      <c r="L1005" s="9"/>
+      <c r="M1005" s="9"/>
+      <c r="N1005" s="9"/>
+      <c r="O1005" s="9"/>
+      <c r="P1005" s="9"/>
+      <c r="Q1005" s="9"/>
+      <c r="R1005" s="9"/>
+      <c r="S1005" s="9"/>
+      <c r="T1005" s="9"/>
+      <c r="U1005" s="9"/>
+      <c r="V1005" s="9"/>
+      <c r="W1005" s="9"/>
+      <c r="X1005" s="9"/>
+      <c r="Y1005" s="9"/>
+      <c r="Z1005" s="9"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>